<commit_message>
fix: 9월 24일 배포
</commit_message>
<xml_diff>
--- a/0_수정 및 추가 사항/250922_소리바로 BO 수정사항.xlsx
+++ b/0_수정 및 추가 사항/250922_소리바로 BO 수정사항.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\new_soribaro_bo\0_수정 및 추가 사항\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13127A21-C331-4798-B740-3F7CF5B0B65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5560CB-8383-4240-BB2D-08C2BC09BD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{59E359C4-9449-4BDC-BEF3-E005F0EC664A}"/>
   </bookViews>
@@ -564,7 +564,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,12 +574,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,7 +633,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -670,9 +664,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
@@ -687,9 +678,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1039,10 +1027,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:3" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -1053,7 +1041,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1061,19 +1049,19 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="11"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1081,13 +1069,13 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="11"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1095,7 +1083,7 @@
       </c>
     </row>
     <row r="10" spans="2:3" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
@@ -1117,7 +1105,7 @@
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1125,13 +1113,13 @@
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="11"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1139,13 +1127,13 @@
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="11"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1153,19 +1141,19 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="11"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="11"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1173,7 +1161,7 @@
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="11"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="5" t="s">
         <v>26</v>
       </c>
@@ -1218,10 +1206,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:3" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -1264,7 +1252,7 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1272,7 +1260,7 @@
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="11"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="5" t="s">
         <v>36</v>
       </c>
@@ -1318,7 +1306,7 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1326,7 +1314,7 @@
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="11"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="5" t="s">
         <v>44</v>
       </c>
@@ -1398,10 +1386,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:3" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -1420,7 +1408,7 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1428,7 +1416,7 @@
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="3" t="s">
         <v>48</v>
       </c>
@@ -1491,10 +1479,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:4" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -1598,11 +1586,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="2:4" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -1739,11 +1727,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="2:4" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -1779,10 +1767,10 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>96</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -1790,8 +1778,8 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="5" t="s">
         <v>98</v>
       </c>
@@ -1843,7 +1831,7 @@
   <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1854,11 +1842,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="2:4" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
@@ -1916,35 +1904,35 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="15" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="5" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>116</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1952,16 +1940,16 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="5" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="14" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1994,10 +1982,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:3" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">

</xml_diff>